<commit_message>
cambio historico y final
</commit_message>
<xml_diff>
--- a/xlsx/a69_f04UPPachuca.xlsx
+++ b/xlsx/a69_f04UPPachuca.xlsx
@@ -333,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -346,9 +346,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -672,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,38 +696,38 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -803,19 +800,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -856,10 +853,10 @@
       <c r="A8" s="3">
         <v>2023</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>44927</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>45291</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -871,28 +868,28 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>45026</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>45026</v>
       </c>
-      <c r="K8" s="7"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2023</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>44927</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>45291</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -904,28 +901,28 @@
       <c r="F9" s="3">
         <v>2</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>45026</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>45026</v>
       </c>
-      <c r="K9" s="7"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2023</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>44927</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>45291</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -937,28 +934,28 @@
       <c r="F10" s="3">
         <v>3</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>45026</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>45026</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2023</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>44927</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>45291</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -970,28 +967,28 @@
       <c r="F11" s="3">
         <v>4</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>45026</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>45026</v>
       </c>
-      <c r="K11" s="7"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2023</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>44927</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>45291</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1003,28 +1000,28 @@
       <c r="F12" s="3">
         <v>5</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>45026</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>45026</v>
       </c>
-      <c r="K12" s="7"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2023</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>44927</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>45291</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1036,97 +1033,19 @@
       <c r="F13" s="3">
         <v>6</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>45026</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>45026</v>
       </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="K13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1152,7 +1071,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:F10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1119,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1214,7 +1133,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1228,7 +1147,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1242,7 +1161,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1256,7 +1175,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1270,7 +1189,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">

</xml_diff>